<commit_message>
Update ImportCitizenData and ImportCitizenModel and migration table
</commit_message>
<xml_diff>
--- a/public/files/mastersample.xlsx
+++ b/public/files/mastersample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\Work\p1\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Local Disk-D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>hhid</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>middle_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>np_first_name</t>
+  </si>
+  <si>
+    <t>np_middle_name</t>
+  </si>
+  <si>
+    <t>np_last_name</t>
+  </si>
+  <si>
+    <t>dob_ad</t>
+  </si>
+  <si>
+    <t>dob_bs</t>
+  </si>
+  <si>
+    <t>citizenship_number</t>
+  </si>
+  <si>
+    <t>issued_date</t>
+  </si>
+  <si>
+    <t>issued_date_ad</t>
+  </si>
+  <si>
+    <t>issued_district_id</t>
+  </si>
+  <si>
+    <t>issued_district_name</t>
+  </si>
+  <si>
+    <t>province_id</t>
+  </si>
+  <si>
+    <t>district_id</t>
+  </si>
+  <si>
+    <t>muncipality_id</t>
+  </si>
+  <si>
+    <t>ward_id</t>
+  </si>
+  <si>
+    <t>tole</t>
+  </si>
   <si>
     <t>f_name</t>
   </si>
@@ -32,88 +89,43 @@
     <t>m_name</t>
   </si>
   <si>
+    <t>g_name</t>
+  </si>
+  <si>
+    <t>citizenship_front</t>
+  </si>
+  <si>
+    <t>citizenship_front_url</t>
+  </si>
+  <si>
+    <t>citizenship_back</t>
+  </si>
+  <si>
+    <t>citizenship_back_url</t>
+  </si>
+  <si>
+    <t>social_security_fund_number</t>
+  </si>
+  <si>
     <t>gender</t>
   </si>
   <si>
-    <t>hhid</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>middle_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>np_first_name</t>
-  </si>
-  <si>
-    <t>np_middle_name</t>
-  </si>
-  <si>
-    <t>np_last_name</t>
-  </si>
-  <si>
-    <t>dob_ad</t>
-  </si>
-  <si>
-    <t>dob_bs</t>
-  </si>
-  <si>
-    <t>citizenship_number</t>
-  </si>
-  <si>
-    <t>issued_date</t>
-  </si>
-  <si>
-    <t>issued_date_ad</t>
-  </si>
-  <si>
-    <t>issued_district_id</t>
-  </si>
-  <si>
-    <t>issued_district_name</t>
-  </si>
-  <si>
-    <t>province_id</t>
-  </si>
-  <si>
-    <t>district_id</t>
-  </si>
-  <si>
-    <t>muncipality_id</t>
-  </si>
-  <si>
-    <t>ward_id</t>
-  </si>
-  <si>
-    <t>tole</t>
-  </si>
-  <si>
-    <t>g_name</t>
-  </si>
-  <si>
-    <t>citizenship_front</t>
-  </si>
-  <si>
-    <t>citizenship_front_url</t>
-  </si>
-  <si>
-    <t>citizenship_back</t>
-  </si>
-  <si>
-    <t>citizenship_back_url</t>
-  </si>
-  <si>
-    <t>social_security_fund_number</t>
-  </si>
-  <si>
     <t>mobile_number</t>
   </si>
   <si>
     <t>email_address</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>ward</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -144,7 +157,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,7 +177,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,131 +458,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" customWidth="1"/>
-    <col min="27" max="27" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>